<commit_message>
Multiple Gabors and mask.
</commit_message>
<xml_diff>
--- a/po-cond01.xlsx
+++ b/po-cond01.xlsx
@@ -528,7 +528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -605,10 +607,10 @@
         <v>1000</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K2">
         <v>12</v>
@@ -652,10 +654,10 @@
         <v>1000</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K3">
         <v>12</v>
@@ -699,10 +701,10 @@
         <v>1000</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K4">
         <v>12</v>
@@ -746,10 +748,10 @@
         <v>1000</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K5">
         <v>12</v>
@@ -793,10 +795,10 @@
         <v>1000</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K6">
         <v>12</v>
@@ -840,10 +842,10 @@
         <v>1000</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K7">
         <v>12</v>
@@ -887,10 +889,10 @@
         <v>1000</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K8">
         <v>12</v>
@@ -934,10 +936,10 @@
         <v>1000</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K9">
         <v>12</v>
@@ -981,10 +983,10 @@
         <v>1000</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K10">
         <v>12</v>
@@ -1028,10 +1030,10 @@
         <v>1000</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K11">
         <v>12</v>
@@ -1075,10 +1077,10 @@
         <v>1000</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K12">
         <v>12</v>
@@ -1122,10 +1124,10 @@
         <v>1000</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K13">
         <v>12</v>
@@ -1169,10 +1171,10 @@
         <v>1000</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K14">
         <v>12</v>
@@ -1216,10 +1218,10 @@
         <v>1000</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K15">
         <v>12</v>

</xml_diff>

<commit_message>
Almost done. Dealt with the onset jitter, frame-to-frame mask updating, orientation discrimination task, and recording the responses to the post-trial questions. Added a data structure d. that contains all of the trial information.
</commit_message>
<xml_diff>
--- a/po-cond01.xlsx
+++ b/po-cond01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="2380" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>condN</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>gabNum</t>
+  </si>
+  <si>
+    <t>jitTmax</t>
   </si>
 </sst>
 </file>
@@ -526,15 +529,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,31 +560,34 @@
         <v>16</v>
       </c>
       <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -604,31 +610,34 @@
         <v>0.01</v>
       </c>
       <c r="H2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K2">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L2">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N2">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -651,31 +660,34 @@
         <v>0.01</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J3">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K3">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L3">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M3">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N3">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -698,31 +710,34 @@
         <v>2.1499999999999998E-2</v>
       </c>
       <c r="H4">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K4">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L4">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M4">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N4">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -745,31 +760,34 @@
         <v>2.1499999999999998E-2</v>
       </c>
       <c r="H5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K5">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L5">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M5">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N5">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O5">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -792,31 +810,34 @@
         <v>4.6399999999999997E-2</v>
       </c>
       <c r="H6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J6">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L6">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M6">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N6">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -839,31 +860,34 @@
         <v>4.6399999999999997E-2</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J7">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K7">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M7">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N7">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O7">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -886,31 +910,34 @@
         <v>0.1</v>
       </c>
       <c r="H8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J8">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L8">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M8">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N8">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -933,31 +960,34 @@
         <v>0.1</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J9">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K9">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L9">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M9">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N9">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O9">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -980,31 +1010,34 @@
         <v>0.21540000000000001</v>
       </c>
       <c r="H10">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J10">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K10">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L10">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M10">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N10">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O10">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1027,31 +1060,34 @@
         <v>0.21540000000000001</v>
       </c>
       <c r="H11">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J11">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K11">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L11">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M11">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N11">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1074,31 +1110,34 @@
         <v>0.4642</v>
       </c>
       <c r="H12">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J12">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K12">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L12">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M12">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N12">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O12">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1121,31 +1160,34 @@
         <v>0.4642</v>
       </c>
       <c r="H13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I13">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J13">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K13">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L13">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M13">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N13">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O13">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1168,31 +1210,34 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K14">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L14">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M14">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N14">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O14">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>1.5</v>
+      </c>
+      <c r="P14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1215,27 +1260,30 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I15">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="J15">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K15">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="L15">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="M15">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="N15">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="O15">
+        <v>1.5</v>
+      </c>
+      <c r="P15">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed the internal circle of gratings, got rid of two levels of pop-out, and implemented prior distributions. Added the individual stats folder.
</commit_message>
<xml_diff>
--- a/po-cond01.xlsx
+++ b/po-cond01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>condN</t>
   </si>
@@ -97,18 +97,6 @@
   </si>
   <si>
     <t>cont5_opp</t>
-  </si>
-  <si>
-    <t>cont6_same</t>
-  </si>
-  <si>
-    <t>cont6_opp</t>
-  </si>
-  <si>
-    <t>cont7_same</t>
-  </si>
-  <si>
-    <t>cont7_opp</t>
   </si>
 </sst>
 </file>
@@ -566,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -629,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
         <v>500</v>
@@ -673,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
         <v>500</v>
@@ -805,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="E6">
         <v>500</v>
@@ -849,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -893,7 +881,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>0.26</v>
+        <v>0.47</v>
       </c>
       <c r="E8">
         <v>500</v>
@@ -937,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>0.26</v>
+        <v>0.47</v>
       </c>
       <c r="E9">
         <v>500</v>
@@ -981,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>0.41</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -1025,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>0.41</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>500</v>
@@ -1062,14 +1050,14 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.64</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>500</v>
@@ -1099,182 +1087,6 @@
         <v>1.5</v>
       </c>
       <c r="N12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>0.64</v>
-      </c>
-      <c r="E13">
-        <v>500</v>
-      </c>
-      <c r="F13">
-        <v>1000</v>
-      </c>
-      <c r="G13">
-        <v>0.5</v>
-      </c>
-      <c r="H13">
-        <v>0.2</v>
-      </c>
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>250</v>
-      </c>
-      <c r="K13">
-        <v>10</v>
-      </c>
-      <c r="L13">
-        <v>6</v>
-      </c>
-      <c r="M13">
-        <v>1.5</v>
-      </c>
-      <c r="N13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>500</v>
-      </c>
-      <c r="F14">
-        <v>1000</v>
-      </c>
-      <c r="G14">
-        <v>0.5</v>
-      </c>
-      <c r="H14">
-        <v>0.2</v>
-      </c>
-      <c r="I14">
-        <v>12</v>
-      </c>
-      <c r="J14">
-        <v>250</v>
-      </c>
-      <c r="K14">
-        <v>10</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>1.5</v>
-      </c>
-      <c r="N14">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>500</v>
-      </c>
-      <c r="F15">
-        <v>1000</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <v>0.2</v>
-      </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>250</v>
-      </c>
-      <c r="K15">
-        <v>10</v>
-      </c>
-      <c r="L15">
-        <v>6</v>
-      </c>
-      <c r="M15">
-        <v>1.5</v>
-      </c>
-      <c r="N15">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>500</v>
-      </c>
-      <c r="F16">
-        <v>1000</v>
-      </c>
-      <c r="G16">
-        <v>0.5</v>
-      </c>
-      <c r="H16">
-        <v>0.2</v>
-      </c>
-      <c r="I16">
-        <v>12</v>
-      </c>
-      <c r="J16">
-        <v>250</v>
-      </c>
-      <c r="K16">
-        <v>10</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>1.5</v>
-      </c>
-      <c r="N16">
         <v>17</v>
       </c>
     </row>

</xml_diff>